<commit_message>
data provider added in test
</commit_message>
<xml_diff>
--- a/src/main/java/com/twitter/testdata/TwitterTestData.xlsx
+++ b/src/main/java/com/twitter/testdata/TwitterTestData.xlsx
@@ -45,13 +45,13 @@
     <t>Tweets</t>
   </si>
   <si>
-    <t>Hello All</t>
-  </si>
-  <si>
-    <t>Good Evening India</t>
-  </si>
-  <si>
-    <t>Automation Framework</t>
+    <t>Hello All Indians</t>
+  </si>
+  <si>
+    <t>Good Evening India and Noida</t>
+  </si>
+  <si>
+    <t>Automation Framework TDD</t>
   </si>
 </sst>
 </file>
@@ -66,6 +66,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -87,6 +88,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -229,12 +231,12 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0255102040816"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -261,7 +263,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>